<commit_message>
Linguistic variable Container implemented.
</commit_message>
<xml_diff>
--- a/Data/Zmienne_lingwistyczne.xlsx
+++ b/Data/Zmienne_lingwistyczne.xlsx
@@ -476,11 +476,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427449320"/>
-        <c:axId val="67064232"/>
+        <c:axId val="188684808"/>
+        <c:axId val="188684416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427449320"/>
+        <c:axId val="188684808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -500,6 +500,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Prędkość waitru  [0.1m/s]  </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.391626345619841"/>
+              <c:y val="0.87868217054263564"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -537,12 +600,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67064232"/>
+        <c:crossAx val="188684416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67064232"/>
+        <c:axId val="188684416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,6 +625,102 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Stopień przynależności</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="1200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.6618357487922701E-3"/>
+              <c:y val="0.19775987303912593"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -599,7 +758,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427449320"/>
+        <c:crossAx val="188684808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -952,11 +1111,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="356068904"/>
-        <c:axId val="356072432"/>
+        <c:axId val="188685200"/>
+        <c:axId val="188685592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="356068904"/>
+        <c:axId val="188685200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -976,6 +1135,82 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Te</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>mperatura w [0.1</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1600" baseline="22000"/>
+                  <a:t>◦</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>C]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.37668173123426335"/>
+              <c:y val="0.84106487547023512"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1013,12 +1248,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="356072432"/>
+        <c:crossAx val="188685592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="356072432"/>
+        <c:axId val="188685592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,6 +1273,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Stopień przynależności</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.2077294685990338E-2"/>
+              <c:y val="0.1999064070479562"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1075,7 +1374,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="356068904"/>
+        <c:crossAx val="188685200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1183,7 +1482,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TG W&amp;J'!$B$4</c:f>
+              <c:f>'TG Z'!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1237,7 +1536,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'TG W&amp;J'!$D$5:$D$8</c:f>
+              <c:f>'TG Z'!$D$5:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1263,7 +1562,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TG W&amp;J'!$B$10</c:f>
+              <c:f>'TG Z'!$B$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1318,7 +1617,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'TG W&amp;J'!$D$11:$D$14</c:f>
+              <c:f>'TG Z'!$D$11:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1344,7 +1643,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TG W&amp;J'!$B$16</c:f>
+              <c:f>'TG Z'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1399,7 +1698,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'TG W&amp;J'!$D$17:$D$21</c:f>
+              <c:f>'TG Z'!$D$17:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1428,11 +1727,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="567548920"/>
-        <c:axId val="567549312"/>
+        <c:axId val="438606856"/>
+        <c:axId val="438607248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="567548920"/>
+        <c:axId val="438606856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1452,6 +1751,82 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Te</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>mperatura w [0.1</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1600" baseline="22000"/>
+                  <a:t>◦</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>C]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.37426546439316888"/>
+              <c:y val="0.84106487547023512"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1489,12 +1864,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567549312"/>
+        <c:crossAx val="438607248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="567549312"/>
+        <c:axId val="438607248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1514,6 +1889,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Stopień przynależności</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.2077338803609255E-2"/>
+              <c:y val="0.18665557748440967"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1551,7 +1990,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567548920"/>
+        <c:crossAx val="438606856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1659,7 +2098,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TG L'!$B$4</c:f>
+              <c:f>'TG Z'!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1713,7 +2152,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'TG L'!$D$5:$D$8</c:f>
+              <c:f>'TG Z'!$D$5:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1739,7 +2178,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TG L'!$B$10</c:f>
+              <c:f>'TG Z'!$B$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1794,7 +2233,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'TG L'!$D$11:$D$14</c:f>
+              <c:f>'TG Z'!$D$11:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1820,7 +2259,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'TG L'!$B$16</c:f>
+              <c:f>'TG Z'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1875,7 +2314,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'TG L'!$D$17:$D$21</c:f>
+              <c:f>'TG Z'!$D$17:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1904,11 +2343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="565258392"/>
-        <c:axId val="565259176"/>
+        <c:axId val="369149912"/>
+        <c:axId val="369150304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="565258392"/>
+        <c:axId val="369149912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1928,6 +2367,82 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Te</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>mperatura w [0.1</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1600" baseline="22000"/>
+                  <a:t>◦</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>C]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.37909799807535782"/>
+              <c:y val="0.84106487547023512"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1965,12 +2480,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565259176"/>
+        <c:crossAx val="369150304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="565259176"/>
+        <c:axId val="369150304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,6 +2505,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Stopień przynależności</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.2077338803609255E-2"/>
+              <c:y val="0.18665557748440967"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2027,7 +2606,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565258392"/>
+        <c:crossAx val="369149912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2380,11 +2959,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427012032"/>
-        <c:axId val="427010856"/>
+        <c:axId val="537434352"/>
+        <c:axId val="537433960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427012032"/>
+        <c:axId val="537434352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2404,6 +2983,77 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Nasłonecznienie [J/cm</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="30000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>]  </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.36719312039685342"/>
+              <c:y val="0.86749983175180023"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2441,12 +3091,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427010856"/>
+        <c:crossAx val="537433960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427010856"/>
+        <c:axId val="537433960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2466,6 +3116,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Stopień przynależności</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.929570670525808E-2"/>
+              <c:y val="0.20343293626758194"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2503,7 +3216,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427012032"/>
+        <c:crossAx val="537434352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5443,19 +6156,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:colOff>287802</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>179363</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5480,19 +6193,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>491837</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>131619</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:colOff>254552</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180056</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5815,7 +6528,7 @@
   <dimension ref="B1:M20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6007,7 +6720,7 @@
   <dimension ref="B1:M20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6196,7 +6909,7 @@
   <dimension ref="B1:M20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6384,8 +7097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M20"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6574,7 +7287,7 @@
   <dimension ref="B1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Linguistic variables improved - report and project
</commit_message>
<xml_diff>
--- a/Data/Zmienne_lingwistyczne.xlsx
+++ b/Data/Zmienne_lingwistyczne.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FG" sheetId="1" r:id="rId1"/>
@@ -272,7 +272,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>21</c:v>
@@ -437,7 +437,7 @@
                   <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>125</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>157</c:v>
@@ -476,11 +476,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188684808"/>
-        <c:axId val="188684416"/>
+        <c:axId val="330447480"/>
+        <c:axId val="330449832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188684808"/>
+        <c:axId val="330447480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,12 +600,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188684416"/>
+        <c:crossAx val="330449832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188684416"/>
+        <c:axId val="330449832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,7 +758,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188684808"/>
+        <c:crossAx val="330447480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -907,7 +907,7 @@
                   <c:v>-81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-60</c:v>
+                  <c:v>-81</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>-10</c:v>
@@ -1072,7 +1072,7 @@
                   <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>270</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>306</c:v>
@@ -1111,11 +1111,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188685200"/>
-        <c:axId val="188685592"/>
+        <c:axId val="330445520"/>
+        <c:axId val="330445912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188685200"/>
+        <c:axId val="330445520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,12 +1248,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188685592"/>
+        <c:crossAx val="330445912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188685592"/>
+        <c:axId val="330445912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1374,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188685200"/>
+        <c:crossAx val="330445520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1523,7 +1523,7 @@
                   <c:v>-81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-50</c:v>
+                  <c:v>-81</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>35</c:v>
@@ -1688,7 +1688,7 @@
                   <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>270</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>306</c:v>
@@ -1727,11 +1727,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="438606856"/>
-        <c:axId val="438607248"/>
+        <c:axId val="330446304"/>
+        <c:axId val="330448656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="438606856"/>
+        <c:axId val="330446304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1864,12 +1864,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438607248"/>
+        <c:crossAx val="330448656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="438607248"/>
+        <c:axId val="330448656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,7 +1990,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438606856"/>
+        <c:crossAx val="330446304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2139,7 +2139,7 @@
                   <c:v>-81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-50</c:v>
+                  <c:v>-81</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -2304,7 +2304,7 @@
                   <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>290</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>306</c:v>
@@ -2343,11 +2343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="369149912"/>
-        <c:axId val="369150304"/>
+        <c:axId val="330446696"/>
+        <c:axId val="330443168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="369149912"/>
+        <c:axId val="330446696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2480,12 +2480,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369150304"/>
+        <c:crossAx val="330443168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="369150304"/>
+        <c:axId val="330443168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2606,7 +2606,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369149912"/>
+        <c:crossAx val="330446696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2755,7 +2755,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>350</c:v>
@@ -2920,7 +2920,7 @@
                   <c:v>1900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2700</c:v>
+                  <c:v>3145</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3145</c:v>
@@ -2959,11 +2959,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="537434352"/>
-        <c:axId val="537433960"/>
+        <c:axId val="332917824"/>
+        <c:axId val="332920960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="537434352"/>
+        <c:axId val="332917824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3091,12 +3091,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="537433960"/>
+        <c:crossAx val="332920960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="537433960"/>
+        <c:axId val="332920960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3216,7 +3216,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="537434352"/>
+        <c:crossAx val="332917824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6528,7 +6528,7 @@
   <dimension ref="B1:M20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6587,7 +6587,7 @@
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -6693,7 +6693,7 @@
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="2">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -6720,7 +6720,7 @@
   <dimension ref="B1:M20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6777,7 +6777,7 @@
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="2">
-        <v>-60</v>
+        <v>-81</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -6882,7 +6882,7 @@
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="2">
-        <v>270</v>
+        <v>306</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -6908,8 +6908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6966,7 +6966,7 @@
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="2">
-        <v>-50</v>
+        <v>-81</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -7071,7 +7071,7 @@
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="2">
-        <v>270</v>
+        <v>306</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -7097,8 +7097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7155,7 +7155,7 @@
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="2">
-        <v>-50</v>
+        <v>-81</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -7260,7 +7260,7 @@
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="2">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -7286,8 +7286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7346,7 +7346,7 @@
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="2">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -7452,7 +7452,7 @@
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="2">
-        <v>2700</v>
+        <v>3145</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
change from tables to equations
</commit_message>
<xml_diff>
--- a/Data/Zmienne_lingwistyczne.xlsx
+++ b/Data/Zmienne_lingwistyczne.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" firstSheet="5" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="FG" sheetId="1" r:id="rId1"/>
@@ -585,11 +585,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="167649040"/>
-        <c:axId val="167644320"/>
+        <c:axId val="131635296"/>
+        <c:axId val="135110496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="167649040"/>
+        <c:axId val="131635296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,12 +709,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167644320"/>
+        <c:crossAx val="135110496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="167644320"/>
+        <c:axId val="135110496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,7 +867,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167649040"/>
+        <c:crossAx val="131635296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1219,11 +1219,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166301000"/>
-        <c:axId val="166304920"/>
+        <c:axId val="434507792"/>
+        <c:axId val="434505048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166301000"/>
+        <c:axId val="434507792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1356,12 +1356,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166304920"/>
+        <c:crossAx val="434505048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166304920"/>
+        <c:axId val="434505048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,7 +1482,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166301000"/>
+        <c:crossAx val="434507792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1835,11 +1835,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166304136"/>
-        <c:axId val="166305704"/>
+        <c:axId val="434505832"/>
+        <c:axId val="434508184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166304136"/>
+        <c:axId val="434505832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1972,12 +1972,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166305704"/>
+        <c:crossAx val="434508184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166305704"/>
+        <c:axId val="434508184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2098,7 +2098,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166304136"/>
+        <c:crossAx val="434505832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2112,7 +2112,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2451,11 +2450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169215504"/>
-        <c:axId val="169216288"/>
+        <c:axId val="434506224"/>
+        <c:axId val="434506616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169215504"/>
+        <c:axId val="434506224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2588,12 +2587,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169216288"/>
+        <c:crossAx val="434506616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169216288"/>
+        <c:axId val="434506616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2714,7 +2713,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169215504"/>
+        <c:crossAx val="434506224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2728,7 +2727,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3067,11 +3065,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169208840"/>
-        <c:axId val="169212368"/>
+        <c:axId val="135111672"/>
+        <c:axId val="135114416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169208840"/>
+        <c:axId val="135111672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3204,12 +3202,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169212368"/>
+        <c:crossAx val="135114416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169212368"/>
+        <c:axId val="135114416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3330,7 +3328,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169208840"/>
+        <c:crossAx val="135111672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3344,7 +3342,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3683,11 +3680,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169215896"/>
-        <c:axId val="169213152"/>
+        <c:axId val="135113240"/>
+        <c:axId val="135115984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169215896"/>
+        <c:axId val="135113240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3820,12 +3817,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169213152"/>
+        <c:crossAx val="135115984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169213152"/>
+        <c:axId val="135115984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3946,7 +3943,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169215896"/>
+        <c:crossAx val="135113240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3960,7 +3957,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4299,11 +4295,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169210016"/>
-        <c:axId val="169214328"/>
+        <c:axId val="435926288"/>
+        <c:axId val="435918840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169210016"/>
+        <c:axId val="435926288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4436,12 +4432,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169214328"/>
+        <c:crossAx val="435918840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169214328"/>
+        <c:axId val="435918840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4562,7 +4558,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169210016"/>
+        <c:crossAx val="435926288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4576,7 +4572,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4915,11 +4910,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169210408"/>
-        <c:axId val="169211192"/>
+        <c:axId val="435924720"/>
+        <c:axId val="435921192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169210408"/>
+        <c:axId val="435924720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5052,12 +5047,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169211192"/>
+        <c:crossAx val="435921192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169211192"/>
+        <c:axId val="435921192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5178,7 +5173,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169210408"/>
+        <c:crossAx val="435924720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5192,7 +5187,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5531,11 +5525,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169211584"/>
-        <c:axId val="169211976"/>
+        <c:axId val="435924328"/>
+        <c:axId val="435925504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169211584"/>
+        <c:axId val="435924328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5663,12 +5657,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169211976"/>
+        <c:crossAx val="435925504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169211976"/>
+        <c:axId val="435925504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5788,7 +5782,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169211584"/>
+        <c:crossAx val="435924328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5802,7 +5796,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6218,11 +6211,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169213544"/>
-        <c:axId val="169725464"/>
+        <c:axId val="435923544"/>
+        <c:axId val="435925896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169213544"/>
+        <c:axId val="435923544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6349,12 +6342,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169725464"/>
+        <c:crossAx val="435925896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169725464"/>
+        <c:axId val="435925896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6507,7 +6500,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169213544"/>
+        <c:crossAx val="435923544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6937,11 +6930,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="167776232"/>
-        <c:axId val="167777800"/>
+        <c:axId val="135108928"/>
+        <c:axId val="135114024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="167776232"/>
+        <c:axId val="135108928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7061,12 +7054,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167777800"/>
+        <c:crossAx val="135114024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="167777800"/>
+        <c:axId val="135114024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7219,7 +7212,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167776232"/>
+        <c:crossAx val="135108928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7233,7 +7226,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7649,11 +7641,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="167775840"/>
-        <c:axId val="167774272"/>
+        <c:axId val="135109712"/>
+        <c:axId val="135115592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="167775840"/>
+        <c:axId val="135109712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7773,12 +7765,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167774272"/>
+        <c:crossAx val="135115592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="167774272"/>
+        <c:axId val="135115592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7931,7 +7923,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167775840"/>
+        <c:crossAx val="135109712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7945,7 +7937,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8361,11 +8352,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="167775056"/>
-        <c:axId val="167775448"/>
+        <c:axId val="135108536"/>
+        <c:axId val="135112456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="167775056"/>
+        <c:axId val="135108536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8485,12 +8476,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167775448"/>
+        <c:crossAx val="135112456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="167775448"/>
+        <c:axId val="135112456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8643,7 +8634,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167775056"/>
+        <c:crossAx val="135108536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8657,7 +8648,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8996,11 +8986,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166306096"/>
-        <c:axId val="166306488"/>
+        <c:axId val="135110104"/>
+        <c:axId val="135111280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166306096"/>
+        <c:axId val="135110104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9133,12 +9123,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166306488"/>
+        <c:crossAx val="135111280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166306488"/>
+        <c:axId val="135111280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9259,7 +9249,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166306096"/>
+        <c:crossAx val="135110104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9611,11 +9601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166302960"/>
-        <c:axId val="166304528"/>
+        <c:axId val="135113632"/>
+        <c:axId val="434508576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166302960"/>
+        <c:axId val="135113632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9748,12 +9738,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166304528"/>
+        <c:crossAx val="434508576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166304528"/>
+        <c:axId val="434508576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9874,7 +9864,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166302960"/>
+        <c:crossAx val="135113632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9888,6 +9878,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10226,11 +10217,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166300216"/>
-        <c:axId val="166307272"/>
+        <c:axId val="434503872"/>
+        <c:axId val="434510536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166300216"/>
+        <c:axId val="434503872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10363,12 +10354,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166307272"/>
+        <c:crossAx val="434510536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166307272"/>
+        <c:axId val="434510536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10489,7 +10480,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166300216"/>
+        <c:crossAx val="434503872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10841,11 +10832,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166301784"/>
-        <c:axId val="166299824"/>
+        <c:axId val="434503088"/>
+        <c:axId val="434507400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166301784"/>
+        <c:axId val="434503088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10978,12 +10969,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166299824"/>
+        <c:crossAx val="434507400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166299824"/>
+        <c:axId val="434507400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11104,7 +11095,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166301784"/>
+        <c:crossAx val="434503088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11457,11 +11448,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166305312"/>
-        <c:axId val="166302176"/>
+        <c:axId val="434510144"/>
+        <c:axId val="434504656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166305312"/>
+        <c:axId val="434510144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11594,12 +11585,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166302176"/>
+        <c:crossAx val="434504656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166302176"/>
+        <c:axId val="434504656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11720,7 +11711,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166305312"/>
+        <c:crossAx val="434510144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -22932,7 +22923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -24447,7 +24438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>

</xml_diff>